<commit_message>
new overall experiment started
</commit_message>
<xml_diff>
--- a/Metadata/result_varyingChgdQRatio.xlsx
+++ b/Metadata/result_varyingChgdQRatio.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J102"/>
+  <dimension ref="A1:J91"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1222,17 +1222,17 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>MDUAL-D</t>
+          <t>SOP</t>
         </is>
       </c>
       <c r="F21" t="n">
-        <v>2910.27</v>
+        <v>51983.87</v>
       </c>
       <c r="G21" t="n">
-        <v>21</v>
+        <v>220.3</v>
       </c>
       <c r="H21" t="n">
-        <v>70</v>
+        <v>319</v>
       </c>
       <c r="I21" t="n">
         <v>313</v>
@@ -1260,17 +1260,17 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>MDUAL-Q</t>
+          <t>pMCSKY</t>
         </is>
       </c>
       <c r="F22" t="n">
-        <v>1025.45</v>
+        <v>52842.81</v>
       </c>
       <c r="G22" t="n">
-        <v>21</v>
+        <v>164.2</v>
       </c>
       <c r="H22" t="n">
-        <v>64</v>
+        <v>266</v>
       </c>
       <c r="I22" t="n">
         <v>313</v>
@@ -1294,27 +1294,27 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>SOP</t>
+          <t>MDUAL</t>
         </is>
       </c>
       <c r="F23" t="n">
-        <v>51983.87</v>
+        <v>2380.05</v>
       </c>
       <c r="G23" t="n">
-        <v>220.3</v>
+        <v>21</v>
       </c>
       <c r="H23" t="n">
-        <v>319</v>
+        <v>59</v>
       </c>
       <c r="I23" t="n">
-        <v>313</v>
+        <v>323</v>
       </c>
       <c r="J23" t="n">
-        <v>615</v>
+        <v>646</v>
       </c>
     </row>
     <row r="24">
@@ -1332,27 +1332,27 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>pMCSKY</t>
+          <t>SOP</t>
         </is>
       </c>
       <c r="F24" t="n">
-        <v>52842.81</v>
+        <v>25678.27</v>
       </c>
       <c r="G24" t="n">
-        <v>164.2</v>
+        <v>222.6</v>
       </c>
       <c r="H24" t="n">
-        <v>266</v>
+        <v>332</v>
       </c>
       <c r="I24" t="n">
-        <v>313</v>
+        <v>323</v>
       </c>
       <c r="J24" t="n">
-        <v>615</v>
+        <v>646</v>
       </c>
     </row>
     <row r="25">
@@ -1374,17 +1374,17 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>MDUAL</t>
+          <t>pMCSKY</t>
         </is>
       </c>
       <c r="F25" t="n">
-        <v>2380.05</v>
+        <v>26204.89</v>
       </c>
       <c r="G25" t="n">
-        <v>21</v>
+        <v>166.5</v>
       </c>
       <c r="H25" t="n">
-        <v>59</v>
+        <v>274</v>
       </c>
       <c r="I25" t="n">
         <v>323</v>
@@ -1408,27 +1408,27 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>SOP</t>
+          <t>MDUAL</t>
         </is>
       </c>
       <c r="F26" t="n">
-        <v>25678.27</v>
+        <v>2428.62</v>
       </c>
       <c r="G26" t="n">
-        <v>222.6</v>
+        <v>21</v>
       </c>
       <c r="H26" t="n">
-        <v>332</v>
+        <v>54</v>
       </c>
       <c r="I26" t="n">
-        <v>323</v>
+        <v>333</v>
       </c>
       <c r="J26" t="n">
-        <v>646</v>
+        <v>714</v>
       </c>
     </row>
     <row r="27">
@@ -1446,27 +1446,27 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>pMCSKY</t>
+          <t>SOP</t>
         </is>
       </c>
       <c r="F27" t="n">
-        <v>26204.89</v>
+        <v>25087.03</v>
       </c>
       <c r="G27" t="n">
-        <v>166.5</v>
+        <v>222.2</v>
       </c>
       <c r="H27" t="n">
-        <v>274</v>
+        <v>328</v>
       </c>
       <c r="I27" t="n">
-        <v>323</v>
+        <v>333</v>
       </c>
       <c r="J27" t="n">
-        <v>646</v>
+        <v>714</v>
       </c>
     </row>
     <row r="28">
@@ -1488,17 +1488,17 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>MDUAL</t>
+          <t>pMCSKY</t>
         </is>
       </c>
       <c r="F28" t="n">
-        <v>2428.62</v>
+        <v>25673.3</v>
       </c>
       <c r="G28" t="n">
-        <v>21</v>
+        <v>166</v>
       </c>
       <c r="H28" t="n">
-        <v>54</v>
+        <v>270</v>
       </c>
       <c r="I28" t="n">
         <v>333</v>
@@ -1522,27 +1522,27 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>SOP</t>
+          <t>MDUAL</t>
         </is>
       </c>
       <c r="F29" t="n">
-        <v>25087.03</v>
+        <v>2475.98</v>
       </c>
       <c r="G29" t="n">
-        <v>222.2</v>
+        <v>21</v>
       </c>
       <c r="H29" t="n">
-        <v>328</v>
+        <v>45</v>
       </c>
       <c r="I29" t="n">
-        <v>333</v>
+        <v>351</v>
       </c>
       <c r="J29" t="n">
-        <v>714</v>
+        <v>736</v>
       </c>
     </row>
     <row r="30">
@@ -1560,27 +1560,27 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>pMCSKY</t>
+          <t>SOP</t>
         </is>
       </c>
       <c r="F30" t="n">
-        <v>25673.3</v>
+        <v>26038.8</v>
       </c>
       <c r="G30" t="n">
-        <v>166</v>
+        <v>223.6</v>
       </c>
       <c r="H30" t="n">
-        <v>270</v>
+        <v>322</v>
       </c>
       <c r="I30" t="n">
-        <v>333</v>
+        <v>351</v>
       </c>
       <c r="J30" t="n">
-        <v>714</v>
+        <v>736</v>
       </c>
     </row>
     <row r="31">
@@ -1602,17 +1602,17 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>MDUAL</t>
+          <t>pMCSKY</t>
         </is>
       </c>
       <c r="F31" t="n">
-        <v>2475.98</v>
+        <v>26698.3</v>
       </c>
       <c r="G31" t="n">
-        <v>21</v>
+        <v>167.5</v>
       </c>
       <c r="H31" t="n">
-        <v>45</v>
+        <v>264</v>
       </c>
       <c r="I31" t="n">
         <v>351</v>
@@ -1627,36 +1627,36 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>FC</t>
+          <t>GAS</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>FC_Q100</t>
+          <t>GAS_Q100</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>SOP</t>
+          <t>MDUAL</t>
         </is>
       </c>
       <c r="F32" t="n">
-        <v>26038.8</v>
+        <v>560.4299999999999</v>
       </c>
       <c r="G32" t="n">
-        <v>223.6</v>
+        <v>19</v>
       </c>
       <c r="H32" t="n">
-        <v>322</v>
+        <v>80</v>
       </c>
       <c r="I32" t="n">
-        <v>351</v>
+        <v>34</v>
       </c>
       <c r="J32" t="n">
-        <v>736</v>
+        <v>83</v>
       </c>
     </row>
     <row r="33">
@@ -1665,36 +1665,36 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>FC</t>
+          <t>GAS</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>FC_Q100</t>
+          <t>GAS_Q100</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>pMCSKY</t>
+          <t>SOP</t>
         </is>
       </c>
       <c r="F33" t="n">
-        <v>26698.3</v>
+        <v>9373.280000000001</v>
       </c>
       <c r="G33" t="n">
-        <v>167.5</v>
+        <v>346.6</v>
       </c>
       <c r="H33" t="n">
-        <v>264</v>
+        <v>419</v>
       </c>
       <c r="I33" t="n">
-        <v>351</v>
+        <v>34</v>
       </c>
       <c r="J33" t="n">
-        <v>736</v>
+        <v>83</v>
       </c>
     </row>
     <row r="34">
@@ -1716,17 +1716,17 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>MDUAL</t>
+          <t>pMCSKY</t>
         </is>
       </c>
       <c r="F34" t="n">
-        <v>560.4299999999999</v>
+        <v>8732.98</v>
       </c>
       <c r="G34" t="n">
-        <v>19</v>
+        <v>303.5</v>
       </c>
       <c r="H34" t="n">
-        <v>80</v>
+        <v>377</v>
       </c>
       <c r="I34" t="n">
         <v>34</v>
@@ -1750,27 +1750,27 @@
         </is>
       </c>
       <c r="D35" t="n">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>SOP</t>
+          <t>MDUAL</t>
         </is>
       </c>
       <c r="F35" t="n">
-        <v>9373.280000000001</v>
+        <v>417.96</v>
       </c>
       <c r="G35" t="n">
-        <v>346.6</v>
+        <v>20.2</v>
       </c>
       <c r="H35" t="n">
-        <v>419</v>
+        <v>80</v>
       </c>
       <c r="I35" t="n">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J35" t="n">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="36">
@@ -1788,27 +1788,27 @@
         </is>
       </c>
       <c r="D36" t="n">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>pMCSKY</t>
+          <t>SOP</t>
         </is>
       </c>
       <c r="F36" t="n">
-        <v>8732.98</v>
+        <v>32568.16</v>
       </c>
       <c r="G36" t="n">
-        <v>303.5</v>
+        <v>373.7</v>
       </c>
       <c r="H36" t="n">
-        <v>377</v>
+        <v>453</v>
       </c>
       <c r="I36" t="n">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J36" t="n">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="37">
@@ -1830,17 +1830,17 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>MDUAL</t>
+          <t>pMCSKY</t>
         </is>
       </c>
       <c r="F37" t="n">
-        <v>417.96</v>
+        <v>32467.03</v>
       </c>
       <c r="G37" t="n">
-        <v>20.2</v>
+        <v>317</v>
       </c>
       <c r="H37" t="n">
-        <v>80</v>
+        <v>396</v>
       </c>
       <c r="I37" t="n">
         <v>32</v>
@@ -1864,27 +1864,27 @@
         </is>
       </c>
       <c r="D38" t="n">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>SOP</t>
+          <t>MDUAL</t>
         </is>
       </c>
       <c r="F38" t="n">
-        <v>32568.16</v>
+        <v>410.73</v>
       </c>
       <c r="G38" t="n">
-        <v>373.7</v>
+        <v>17.9</v>
       </c>
       <c r="H38" t="n">
-        <v>453</v>
+        <v>78</v>
       </c>
       <c r="I38" t="n">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="J38" t="n">
-        <v>79</v>
+        <v>93</v>
       </c>
     </row>
     <row r="39">
@@ -1902,27 +1902,27 @@
         </is>
       </c>
       <c r="D39" t="n">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>pMCSKY</t>
+          <t>SOP</t>
         </is>
       </c>
       <c r="F39" t="n">
-        <v>32467.03</v>
+        <v>31853.05</v>
       </c>
       <c r="G39" t="n">
-        <v>317</v>
+        <v>371.1</v>
       </c>
       <c r="H39" t="n">
-        <v>396</v>
+        <v>458</v>
       </c>
       <c r="I39" t="n">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="J39" t="n">
-        <v>79</v>
+        <v>93</v>
       </c>
     </row>
     <row r="40">
@@ -1944,17 +1944,17 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>MDUAL</t>
+          <t>pMCSKY</t>
         </is>
       </c>
       <c r="F40" t="n">
-        <v>410.73</v>
+        <v>31742.56</v>
       </c>
       <c r="G40" t="n">
-        <v>17.9</v>
+        <v>312.5</v>
       </c>
       <c r="H40" t="n">
-        <v>78</v>
+        <v>396</v>
       </c>
       <c r="I40" t="n">
         <v>41</v>
@@ -1978,27 +1978,27 @@
         </is>
       </c>
       <c r="D41" t="n">
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>SOP</t>
+          <t>MDUAL</t>
         </is>
       </c>
       <c r="F41" t="n">
-        <v>31853.05</v>
+        <v>516.11</v>
       </c>
       <c r="G41" t="n">
-        <v>371.1</v>
+        <v>20</v>
       </c>
       <c r="H41" t="n">
-        <v>458</v>
+        <v>80</v>
       </c>
       <c r="I41" t="n">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J41" t="n">
-        <v>93</v>
+        <v>112</v>
       </c>
     </row>
     <row r="42">
@@ -2016,27 +2016,27 @@
         </is>
       </c>
       <c r="D42" t="n">
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>pMCSKY</t>
+          <t>SOP</t>
         </is>
       </c>
       <c r="F42" t="n">
-        <v>31742.56</v>
+        <v>32355.13</v>
       </c>
       <c r="G42" t="n">
-        <v>312.5</v>
+        <v>363.8</v>
       </c>
       <c r="H42" t="n">
-        <v>396</v>
+        <v>457</v>
       </c>
       <c r="I42" t="n">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J42" t="n">
-        <v>93</v>
+        <v>112</v>
       </c>
     </row>
     <row r="43">
@@ -2058,17 +2058,17 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>MDUAL</t>
+          <t>pMCSKY</t>
         </is>
       </c>
       <c r="F43" t="n">
-        <v>516.11</v>
+        <v>32128.16</v>
       </c>
       <c r="G43" t="n">
-        <v>20</v>
+        <v>303.9</v>
       </c>
       <c r="H43" t="n">
-        <v>80</v>
+        <v>401</v>
       </c>
       <c r="I43" t="n">
         <v>40</v>
@@ -2092,27 +2092,27 @@
         </is>
       </c>
       <c r="D44" t="n">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>SOP</t>
+          <t>MDUAL</t>
         </is>
       </c>
       <c r="F44" t="n">
-        <v>32355.13</v>
+        <v>454.16</v>
       </c>
       <c r="G44" t="n">
-        <v>363.8</v>
+        <v>16.7</v>
       </c>
       <c r="H44" t="n">
-        <v>457</v>
+        <v>80</v>
       </c>
       <c r="I44" t="n">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="J44" t="n">
-        <v>112</v>
+        <v>86</v>
       </c>
     </row>
     <row r="45">
@@ -2130,27 +2130,27 @@
         </is>
       </c>
       <c r="D45" t="n">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>pMCSKY</t>
+          <t>SOP</t>
         </is>
       </c>
       <c r="F45" t="n">
-        <v>32128.16</v>
+        <v>32009.18</v>
       </c>
       <c r="G45" t="n">
-        <v>303.9</v>
+        <v>361.6</v>
       </c>
       <c r="H45" t="n">
-        <v>401</v>
+        <v>448</v>
       </c>
       <c r="I45" t="n">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="J45" t="n">
-        <v>112</v>
+        <v>86</v>
       </c>
     </row>
     <row r="46">
@@ -2172,17 +2172,17 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>MDUAL</t>
+          <t>pMCSKY</t>
         </is>
       </c>
       <c r="F46" t="n">
-        <v>454.16</v>
+        <v>31955.34</v>
       </c>
       <c r="G46" t="n">
-        <v>16.7</v>
+        <v>302.6</v>
       </c>
       <c r="H46" t="n">
-        <v>80</v>
+        <v>392</v>
       </c>
       <c r="I46" t="n">
         <v>32</v>
@@ -2197,36 +2197,36 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>GAS</t>
+          <t>HPC</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>GAS_Q100</t>
+          <t>HPC_Q100</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>SOP</t>
+          <t>MDUAL</t>
         </is>
       </c>
       <c r="F47" t="n">
-        <v>32009.18</v>
+        <v>253.8</v>
       </c>
       <c r="G47" t="n">
-        <v>361.6</v>
+        <v>11.7</v>
       </c>
       <c r="H47" t="n">
-        <v>448</v>
+        <v>31.5</v>
       </c>
       <c r="I47" t="n">
-        <v>32</v>
+        <v>93.5</v>
       </c>
       <c r="J47" t="n">
-        <v>86</v>
+        <v>285.5</v>
       </c>
     </row>
     <row r="48">
@@ -2235,36 +2235,36 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>GAS</t>
+          <t>HPC</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>GAS_Q100</t>
+          <t>HPC_Q100</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>pMCSKY</t>
+          <t>SOP</t>
         </is>
       </c>
       <c r="F48" t="n">
-        <v>31955.34</v>
+        <v>2211.135</v>
       </c>
       <c r="G48" t="n">
-        <v>302.6</v>
+        <v>138.75</v>
       </c>
       <c r="H48" t="n">
-        <v>392</v>
+        <v>193.5</v>
       </c>
       <c r="I48" t="n">
-        <v>32</v>
+        <v>93.5</v>
       </c>
       <c r="J48" t="n">
-        <v>86</v>
+        <v>285.5</v>
       </c>
     </row>
     <row r="49">
@@ -2286,17 +2286,17 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>MDUAL</t>
+          <t>pMCSKY</t>
         </is>
       </c>
       <c r="F49" t="n">
-        <v>253.8</v>
+        <v>2058.805</v>
       </c>
       <c r="G49" t="n">
-        <v>11.7</v>
+        <v>96.34999999999999</v>
       </c>
       <c r="H49" t="n">
-        <v>31.5</v>
+        <v>156.5</v>
       </c>
       <c r="I49" t="n">
         <v>93.5</v>
@@ -2320,27 +2320,27 @@
         </is>
       </c>
       <c r="D50" t="n">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>SOP</t>
+          <t>MDUAL</t>
         </is>
       </c>
       <c r="F50" t="n">
-        <v>2211.135</v>
+        <v>257.924</v>
       </c>
       <c r="G50" t="n">
-        <v>138.75</v>
+        <v>10.16</v>
       </c>
       <c r="H50" t="n">
-        <v>193.5</v>
+        <v>31.8</v>
       </c>
       <c r="I50" t="n">
-        <v>93.5</v>
+        <v>97.2</v>
       </c>
       <c r="J50" t="n">
-        <v>285.5</v>
+        <v>251.8</v>
       </c>
     </row>
     <row r="51">
@@ -2358,27 +2358,27 @@
         </is>
       </c>
       <c r="D51" t="n">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>pMCSKY</t>
+          <t>SOP</t>
         </is>
       </c>
       <c r="F51" t="n">
-        <v>2058.805</v>
+        <v>6579.101999999999</v>
       </c>
       <c r="G51" t="n">
-        <v>96.34999999999999</v>
+        <v>142.98</v>
       </c>
       <c r="H51" t="n">
-        <v>156.5</v>
+        <v>205.8</v>
       </c>
       <c r="I51" t="n">
-        <v>93.5</v>
+        <v>97.2</v>
       </c>
       <c r="J51" t="n">
-        <v>285.5</v>
+        <v>251.8</v>
       </c>
     </row>
     <row r="52">
@@ -2400,17 +2400,17 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>MDUAL</t>
+          <t>pMCSKY</t>
         </is>
       </c>
       <c r="F52" t="n">
-        <v>257.924</v>
+        <v>6093.838</v>
       </c>
       <c r="G52" t="n">
-        <v>10.16</v>
+        <v>78.42</v>
       </c>
       <c r="H52" t="n">
-        <v>31.8</v>
+        <v>142.2</v>
       </c>
       <c r="I52" t="n">
         <v>97.2</v>
@@ -2434,27 +2434,27 @@
         </is>
       </c>
       <c r="D53" t="n">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>MDUAL-D</t>
+          <t>MDUAL</t>
         </is>
       </c>
       <c r="F53" t="n">
-        <v>2262.212</v>
+        <v>217.19</v>
       </c>
       <c r="G53" t="n">
-        <v>9.26</v>
+        <v>10.2</v>
       </c>
       <c r="H53" t="n">
-        <v>31.2</v>
+        <v>32</v>
       </c>
       <c r="I53" t="n">
-        <v>97.2</v>
+        <v>91</v>
       </c>
       <c r="J53" t="n">
-        <v>251.8</v>
+        <v>231</v>
       </c>
     </row>
     <row r="54">
@@ -2472,27 +2472,27 @@
         </is>
       </c>
       <c r="D54" t="n">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>MDUAL-Q</t>
+          <t>SOP</t>
         </is>
       </c>
       <c r="F54" t="n">
-        <v>349.0559999999999</v>
+        <v>5830.33</v>
       </c>
       <c r="G54" t="n">
-        <v>11.7</v>
+        <v>142.85</v>
       </c>
       <c r="H54" t="n">
-        <v>33</v>
+        <v>199</v>
       </c>
       <c r="I54" t="n">
-        <v>97.2</v>
+        <v>94.5</v>
       </c>
       <c r="J54" t="n">
-        <v>251.8</v>
+        <v>240.5</v>
       </c>
     </row>
     <row r="55">
@@ -2510,27 +2510,27 @@
         </is>
       </c>
       <c r="D55" t="n">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>NAIVE</t>
+          <t>pMCSKY</t>
         </is>
       </c>
       <c r="F55" t="n">
-        <v>20947.972</v>
+        <v>5595.19</v>
       </c>
       <c r="G55" t="n">
-        <v>2.48</v>
+        <v>77.8</v>
       </c>
       <c r="H55" t="n">
-        <v>22</v>
+        <v>133</v>
       </c>
       <c r="I55" t="n">
-        <v>97.2</v>
+        <v>91</v>
       </c>
       <c r="J55" t="n">
-        <v>251.8</v>
+        <v>231</v>
       </c>
     </row>
     <row r="56">
@@ -2548,27 +2548,27 @@
         </is>
       </c>
       <c r="D56" t="n">
-        <v>0.2</v>
+        <v>0.8</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>SOP</t>
+          <t>MDUAL</t>
         </is>
       </c>
       <c r="F56" t="n">
-        <v>6579.101999999999</v>
+        <v>232.54</v>
       </c>
       <c r="G56" t="n">
-        <v>142.98</v>
+        <v>10.2</v>
       </c>
       <c r="H56" t="n">
-        <v>205.8</v>
+        <v>33</v>
       </c>
       <c r="I56" t="n">
-        <v>97.2</v>
+        <v>95</v>
       </c>
       <c r="J56" t="n">
-        <v>251.8</v>
+        <v>241</v>
       </c>
     </row>
     <row r="57">
@@ -2586,27 +2586,27 @@
         </is>
       </c>
       <c r="D57" t="n">
-        <v>0.2</v>
+        <v>0.8</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>pMCSKY</t>
+          <t>SOP</t>
         </is>
       </c>
       <c r="F57" t="n">
-        <v>6093.838</v>
+        <v>5838.28</v>
       </c>
       <c r="G57" t="n">
-        <v>78.42</v>
+        <v>143.2</v>
       </c>
       <c r="H57" t="n">
-        <v>142.2</v>
+        <v>206</v>
       </c>
       <c r="I57" t="n">
-        <v>97.2</v>
+        <v>95</v>
       </c>
       <c r="J57" t="n">
-        <v>251.8</v>
+        <v>241</v>
       </c>
     </row>
     <row r="58">
@@ -2624,27 +2624,27 @@
         </is>
       </c>
       <c r="D58" t="n">
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>MDUAL</t>
+          <t>pMCSKY</t>
         </is>
       </c>
       <c r="F58" t="n">
-        <v>217.19</v>
+        <v>5603.52</v>
       </c>
       <c r="G58" t="n">
-        <v>10.2</v>
+        <v>78.09999999999999</v>
       </c>
       <c r="H58" t="n">
-        <v>32</v>
+        <v>149</v>
       </c>
       <c r="I58" t="n">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="J58" t="n">
-        <v>231</v>
+        <v>241</v>
       </c>
     </row>
     <row r="59">
@@ -2662,27 +2662,27 @@
         </is>
       </c>
       <c r="D59" t="n">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>SOP</t>
+          <t>MDUAL</t>
         </is>
       </c>
       <c r="F59" t="n">
-        <v>5830.33</v>
+        <v>230.24</v>
       </c>
       <c r="G59" t="n">
-        <v>142.85</v>
+        <v>10.1</v>
       </c>
       <c r="H59" t="n">
-        <v>199</v>
+        <v>32</v>
       </c>
       <c r="I59" t="n">
-        <v>94.5</v>
+        <v>99</v>
       </c>
       <c r="J59" t="n">
-        <v>240.5</v>
+        <v>243</v>
       </c>
     </row>
     <row r="60">
@@ -2700,27 +2700,27 @@
         </is>
       </c>
       <c r="D60" t="n">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>pMCSKY</t>
+          <t>SOP</t>
         </is>
       </c>
       <c r="F60" t="n">
-        <v>5595.19</v>
+        <v>5847.93</v>
       </c>
       <c r="G60" t="n">
-        <v>77.8</v>
+        <v>143.2</v>
       </c>
       <c r="H60" t="n">
-        <v>133</v>
+        <v>207</v>
       </c>
       <c r="I60" t="n">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="J60" t="n">
-        <v>231</v>
+        <v>243</v>
       </c>
     </row>
     <row r="61">
@@ -2738,27 +2738,27 @@
         </is>
       </c>
       <c r="D61" t="n">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>MDUAL</t>
+          <t>pMCSKY</t>
         </is>
       </c>
       <c r="F61" t="n">
-        <v>232.54</v>
+        <v>5527.89</v>
       </c>
       <c r="G61" t="n">
-        <v>10.2</v>
+        <v>77.8</v>
       </c>
       <c r="H61" t="n">
-        <v>33</v>
+        <v>142</v>
       </c>
       <c r="I61" t="n">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="J61" t="n">
-        <v>241</v>
+        <v>243</v>
       </c>
     </row>
     <row r="62">
@@ -2767,36 +2767,36 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>HPC</t>
+          <t>STK</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>HPC_Q100</t>
+          <t>STK_Q100</t>
         </is>
       </c>
       <c r="D62" t="n">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>SOP</t>
+          <t>MDUAL</t>
         </is>
       </c>
       <c r="F62" t="n">
-        <v>5838.28</v>
+        <v>13.986</v>
       </c>
       <c r="G62" t="n">
-        <v>143.2</v>
+        <v>4.2</v>
       </c>
       <c r="H62" t="n">
-        <v>206</v>
+        <v>9.199999999999999</v>
       </c>
       <c r="I62" t="n">
-        <v>95</v>
+        <v>60.8</v>
       </c>
       <c r="J62" t="n">
-        <v>241</v>
+        <v>217.2</v>
       </c>
     </row>
     <row r="63">
@@ -2805,36 +2805,36 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>HPC</t>
+          <t>STK</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>HPC_Q100</t>
+          <t>STK_Q100</t>
         </is>
       </c>
       <c r="D63" t="n">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>pMCSKY</t>
+          <t>SOP</t>
         </is>
       </c>
       <c r="F63" t="n">
-        <v>5603.52</v>
+        <v>5314.8</v>
       </c>
       <c r="G63" t="n">
-        <v>78.09999999999999</v>
+        <v>167.52</v>
       </c>
       <c r="H63" t="n">
-        <v>149</v>
+        <v>174.4</v>
       </c>
       <c r="I63" t="n">
-        <v>95</v>
+        <v>60.8</v>
       </c>
       <c r="J63" t="n">
-        <v>241</v>
+        <v>217.2</v>
       </c>
     </row>
     <row r="64">
@@ -2843,36 +2843,36 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>HPC</t>
+          <t>STK</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>HPC_Q100</t>
+          <t>STK_Q100</t>
         </is>
       </c>
       <c r="D64" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>MDUAL</t>
+          <t>pMCSKY</t>
         </is>
       </c>
       <c r="F64" t="n">
-        <v>230.24</v>
+        <v>4956.232</v>
       </c>
       <c r="G64" t="n">
-        <v>10.1</v>
+        <v>124.64</v>
       </c>
       <c r="H64" t="n">
-        <v>32</v>
+        <v>131.8</v>
       </c>
       <c r="I64" t="n">
-        <v>99</v>
+        <v>60.8</v>
       </c>
       <c r="J64" t="n">
-        <v>243</v>
+        <v>217.2</v>
       </c>
     </row>
     <row r="65">
@@ -2881,36 +2881,36 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>HPC</t>
+          <t>STK</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>HPC_Q100</t>
+          <t>STK_Q100</t>
         </is>
       </c>
       <c r="D65" t="n">
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>SOP</t>
+          <t>MDUAL</t>
         </is>
       </c>
       <c r="F65" t="n">
-        <v>5847.93</v>
+        <v>16.966</v>
       </c>
       <c r="G65" t="n">
-        <v>143.2</v>
+        <v>4</v>
       </c>
       <c r="H65" t="n">
-        <v>207</v>
+        <v>9.199999999999999</v>
       </c>
       <c r="I65" t="n">
-        <v>99</v>
+        <v>74.2</v>
       </c>
       <c r="J65" t="n">
-        <v>243</v>
+        <v>239.6</v>
       </c>
     </row>
     <row r="66">
@@ -2919,36 +2919,36 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>HPC</t>
+          <t>STK</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>HPC_Q100</t>
+          <t>STK_Q100</t>
         </is>
       </c>
       <c r="D66" t="n">
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>pMCSKY</t>
+          <t>SOP</t>
         </is>
       </c>
       <c r="F66" t="n">
-        <v>5527.89</v>
+        <v>17103.862</v>
       </c>
       <c r="G66" t="n">
-        <v>77.8</v>
+        <v>179.82</v>
       </c>
       <c r="H66" t="n">
-        <v>142</v>
+        <v>188.6</v>
       </c>
       <c r="I66" t="n">
-        <v>99</v>
+        <v>74.2</v>
       </c>
       <c r="J66" t="n">
-        <v>243</v>
+        <v>239.6</v>
       </c>
     </row>
     <row r="67">
@@ -2966,27 +2966,27 @@
         </is>
       </c>
       <c r="D67" t="n">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>MDUAL</t>
+          <t>pMCSKY</t>
         </is>
       </c>
       <c r="F67" t="n">
-        <v>22.048</v>
+        <v>16510.908</v>
       </c>
       <c r="G67" t="n">
-        <v>4.12</v>
+        <v>120.32</v>
       </c>
       <c r="H67" t="n">
-        <v>10</v>
+        <v>130.6</v>
       </c>
       <c r="I67" t="n">
-        <v>97.2</v>
+        <v>74.2</v>
       </c>
       <c r="J67" t="n">
-        <v>292.8</v>
+        <v>239.6</v>
       </c>
     </row>
     <row r="68">
@@ -3004,27 +3004,27 @@
         </is>
       </c>
       <c r="D68" t="n">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>SOP</t>
+          <t>MDUAL</t>
         </is>
       </c>
       <c r="F68" t="n">
-        <v>3286.796</v>
+        <v>18.418</v>
       </c>
       <c r="G68" t="n">
-        <v>173.74</v>
+        <v>4</v>
       </c>
       <c r="H68" t="n">
-        <v>196.2</v>
+        <v>9</v>
       </c>
       <c r="I68" t="n">
-        <v>97.2</v>
+        <v>73.2</v>
       </c>
       <c r="J68" t="n">
-        <v>292.8</v>
+        <v>251.2</v>
       </c>
     </row>
     <row r="69">
@@ -3042,27 +3042,27 @@
         </is>
       </c>
       <c r="D69" t="n">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>pMCSKY</t>
+          <t>SOP</t>
         </is>
       </c>
       <c r="F69" t="n">
-        <v>3156.284</v>
+        <v>18188.106</v>
       </c>
       <c r="G69" t="n">
-        <v>132.36</v>
+        <v>180.76</v>
       </c>
       <c r="H69" t="n">
-        <v>155.2</v>
+        <v>189.6</v>
       </c>
       <c r="I69" t="n">
-        <v>97.2</v>
+        <v>73.2</v>
       </c>
       <c r="J69" t="n">
-        <v>292.8</v>
+        <v>251.2</v>
       </c>
     </row>
     <row r="70">
@@ -3080,27 +3080,27 @@
         </is>
       </c>
       <c r="D70" t="n">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>MDUAL</t>
+          <t>pMCSKY</t>
         </is>
       </c>
       <c r="F70" t="n">
-        <v>23.184</v>
+        <v>16770.242</v>
       </c>
       <c r="G70" t="n">
-        <v>4</v>
+        <v>121.92</v>
       </c>
       <c r="H70" t="n">
-        <v>11.2</v>
+        <v>132.4</v>
       </c>
       <c r="I70" t="n">
-        <v>86.2</v>
+        <v>73.2</v>
       </c>
       <c r="J70" t="n">
-        <v>278.2</v>
+        <v>251.2</v>
       </c>
     </row>
     <row r="71">
@@ -3118,27 +3118,27 @@
         </is>
       </c>
       <c r="D71" t="n">
-        <v>0.2</v>
+        <v>0.8</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>MDUAL-D</t>
+          <t>MDUAL</t>
         </is>
       </c>
       <c r="F71" t="n">
-        <v>67.776</v>
+        <v>19.104</v>
       </c>
       <c r="G71" t="n">
         <v>4</v>
       </c>
       <c r="H71" t="n">
-        <v>11.4</v>
+        <v>9.199999999999999</v>
       </c>
       <c r="I71" t="n">
-        <v>86.2</v>
+        <v>74.2</v>
       </c>
       <c r="J71" t="n">
-        <v>278.2</v>
+        <v>248.6</v>
       </c>
     </row>
     <row r="72">
@@ -3156,27 +3156,27 @@
         </is>
       </c>
       <c r="D72" t="n">
-        <v>0.2</v>
+        <v>0.8</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>MDUAL-Q</t>
+          <t>SOP</t>
         </is>
       </c>
       <c r="F72" t="n">
-        <v>769.878</v>
+        <v>17486.254</v>
       </c>
       <c r="G72" t="n">
-        <v>4</v>
+        <v>179.78</v>
       </c>
       <c r="H72" t="n">
-        <v>11</v>
+        <v>188.2</v>
       </c>
       <c r="I72" t="n">
-        <v>86.2</v>
+        <v>74.2</v>
       </c>
       <c r="J72" t="n">
-        <v>278.2</v>
+        <v>248.6</v>
       </c>
     </row>
     <row r="73">
@@ -3194,27 +3194,27 @@
         </is>
       </c>
       <c r="D73" t="n">
-        <v>0.2</v>
+        <v>0.8</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>NAIVE</t>
+          <t>pMCSKY</t>
         </is>
       </c>
       <c r="F73" t="n">
-        <v>16013.69</v>
+        <v>16494.296</v>
       </c>
       <c r="G73" t="n">
-        <v>2</v>
+        <v>119.48</v>
       </c>
       <c r="H73" t="n">
-        <v>8</v>
+        <v>130.2</v>
       </c>
       <c r="I73" t="n">
-        <v>86.2</v>
+        <v>74.2</v>
       </c>
       <c r="J73" t="n">
-        <v>278.2</v>
+        <v>248.6</v>
       </c>
     </row>
     <row r="74">
@@ -3232,27 +3232,27 @@
         </is>
       </c>
       <c r="D74" t="n">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>SOP</t>
+          <t>MDUAL</t>
         </is>
       </c>
       <c r="F74" t="n">
-        <v>13180.518</v>
+        <v>19.236</v>
       </c>
       <c r="G74" t="n">
-        <v>179.58</v>
+        <v>4</v>
       </c>
       <c r="H74" t="n">
-        <v>250.2</v>
+        <v>9.6</v>
       </c>
       <c r="I74" t="n">
-        <v>86.2</v>
+        <v>66</v>
       </c>
       <c r="J74" t="n">
-        <v>278.2</v>
+        <v>253.6</v>
       </c>
     </row>
     <row r="75">
@@ -3270,27 +3270,27 @@
         </is>
       </c>
       <c r="D75" t="n">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>pMCSKY</t>
+          <t>SOP</t>
         </is>
       </c>
       <c r="F75" t="n">
-        <v>12634.7</v>
+        <v>18074</v>
       </c>
       <c r="G75" t="n">
-        <v>121.1</v>
+        <v>180.46</v>
       </c>
       <c r="H75" t="n">
-        <v>150.8</v>
+        <v>188.8</v>
       </c>
       <c r="I75" t="n">
-        <v>86.2</v>
+        <v>66</v>
       </c>
       <c r="J75" t="n">
-        <v>278.2</v>
+        <v>253.6</v>
       </c>
     </row>
     <row r="76">
@@ -3308,27 +3308,27 @@
         </is>
       </c>
       <c r="D76" t="n">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>MDUAL</t>
+          <t>pMCSKY</t>
         </is>
       </c>
       <c r="F76" t="n">
-        <v>24.042</v>
+        <v>16946.358</v>
       </c>
       <c r="G76" t="n">
-        <v>4</v>
+        <v>121.9</v>
       </c>
       <c r="H76" t="n">
-        <v>11.6</v>
+        <v>131.2</v>
       </c>
       <c r="I76" t="n">
-        <v>88.2</v>
+        <v>66</v>
       </c>
       <c r="J76" t="n">
-        <v>279.4</v>
+        <v>253.6</v>
       </c>
     </row>
     <row r="77">
@@ -3337,36 +3337,36 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>STK</t>
+          <t>TAO</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>STK_Q100</t>
+          <t>TAO_Q100</t>
         </is>
       </c>
       <c r="D77" t="n">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>SOP</t>
+          <t>MDUAL</t>
         </is>
       </c>
       <c r="F77" t="n">
-        <v>13157.826</v>
+        <v>100.0466666666667</v>
       </c>
       <c r="G77" t="n">
-        <v>179.4</v>
+        <v>6.099999999999999</v>
       </c>
       <c r="H77" t="n">
-        <v>260.6</v>
+        <v>16</v>
       </c>
       <c r="I77" t="n">
-        <v>88.2</v>
+        <v>116</v>
       </c>
       <c r="J77" t="n">
-        <v>279.4</v>
+        <v>505.6666666666667</v>
       </c>
     </row>
     <row r="78">
@@ -3375,36 +3375,36 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>STK</t>
+          <t>TAO</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>STK_Q100</t>
+          <t>TAO_Q100</t>
         </is>
       </c>
       <c r="D78" t="n">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>pMCSKY</t>
+          <t>SOP</t>
         </is>
       </c>
       <c r="F78" t="n">
-        <v>12882.892</v>
+        <v>4565.05</v>
       </c>
       <c r="G78" t="n">
-        <v>121.16</v>
+        <v>228.1</v>
       </c>
       <c r="H78" t="n">
-        <v>156.2</v>
+        <v>267</v>
       </c>
       <c r="I78" t="n">
-        <v>88.2</v>
+        <v>116</v>
       </c>
       <c r="J78" t="n">
-        <v>279.4</v>
+        <v>505.6666666666667</v>
       </c>
     </row>
     <row r="79">
@@ -3413,36 +3413,36 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>STK</t>
+          <t>TAO</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>STK_Q100</t>
+          <t>TAO_Q100</t>
         </is>
       </c>
       <c r="D79" t="n">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>MDUAL</t>
+          <t>pMCSKY</t>
         </is>
       </c>
       <c r="F79" t="n">
-        <v>25.112</v>
+        <v>4428.433333333333</v>
       </c>
       <c r="G79" t="n">
-        <v>4</v>
+        <v>186.7666666666667</v>
       </c>
       <c r="H79" t="n">
-        <v>11.4</v>
+        <v>226</v>
       </c>
       <c r="I79" t="n">
-        <v>87.40000000000001</v>
+        <v>116</v>
       </c>
       <c r="J79" t="n">
-        <v>277.2</v>
+        <v>505.6666666666667</v>
       </c>
     </row>
     <row r="80">
@@ -3451,36 +3451,36 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>STK</t>
+          <t>TAO</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>STK_Q100</t>
+          <t>TAO_Q100</t>
         </is>
       </c>
       <c r="D80" t="n">
-        <v>0.8</v>
+        <v>0.2</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>SOP</t>
+          <t>MDUAL</t>
         </is>
       </c>
       <c r="F80" t="n">
-        <v>12985.364</v>
+        <v>109.536</v>
       </c>
       <c r="G80" t="n">
-        <v>179.72</v>
+        <v>6.26</v>
       </c>
       <c r="H80" t="n">
-        <v>207.6</v>
+        <v>18.4</v>
       </c>
       <c r="I80" t="n">
-        <v>87.40000000000001</v>
+        <v>121.6</v>
       </c>
       <c r="J80" t="n">
-        <v>277.2</v>
+        <v>560.2</v>
       </c>
     </row>
     <row r="81">
@@ -3489,36 +3489,36 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>STK</t>
+          <t>TAO</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>STK_Q100</t>
+          <t>TAO_Q100</t>
         </is>
       </c>
       <c r="D81" t="n">
-        <v>0.8</v>
+        <v>0.2</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>pMCSKY</t>
+          <t>SOP</t>
         </is>
       </c>
       <c r="F81" t="n">
-        <v>12801.982</v>
+        <v>24179.346</v>
       </c>
       <c r="G81" t="n">
-        <v>121.64</v>
+        <v>229.84</v>
       </c>
       <c r="H81" t="n">
-        <v>152</v>
+        <v>279.2</v>
       </c>
       <c r="I81" t="n">
-        <v>87.40000000000001</v>
+        <v>121.6</v>
       </c>
       <c r="J81" t="n">
-        <v>277.2</v>
+        <v>560.2</v>
       </c>
     </row>
     <row r="82">
@@ -3527,36 +3527,36 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>STK</t>
+          <t>TAO</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>STK_Q100</t>
+          <t>TAO_Q100</t>
         </is>
       </c>
       <c r="D82" t="n">
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>MDUAL</t>
+          <t>pMCSKY</t>
         </is>
       </c>
       <c r="F82" t="n">
-        <v>24.766</v>
+        <v>23755.652</v>
       </c>
       <c r="G82" t="n">
-        <v>4</v>
+        <v>170.6</v>
       </c>
       <c r="H82" t="n">
-        <v>12</v>
+        <v>220</v>
       </c>
       <c r="I82" t="n">
-        <v>88.59999999999999</v>
+        <v>121.6</v>
       </c>
       <c r="J82" t="n">
-        <v>283</v>
+        <v>560.2</v>
       </c>
     </row>
     <row r="83">
@@ -3565,36 +3565,36 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>STK</t>
+          <t>TAO</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>STK_Q100</t>
+          <t>TAO_Q100</t>
         </is>
       </c>
       <c r="D83" t="n">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>SOP</t>
+          <t>MDUAL</t>
         </is>
       </c>
       <c r="F83" t="n">
-        <v>13007.05</v>
+        <v>117.3966666666667</v>
       </c>
       <c r="G83" t="n">
-        <v>179.68</v>
+        <v>6.333333333333333</v>
       </c>
       <c r="H83" t="n">
-        <v>208.2</v>
+        <v>19</v>
       </c>
       <c r="I83" t="n">
-        <v>88.59999999999999</v>
+        <v>122.3333333333333</v>
       </c>
       <c r="J83" t="n">
-        <v>283</v>
+        <v>564</v>
       </c>
     </row>
     <row r="84">
@@ -3603,36 +3603,36 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>STK</t>
+          <t>TAO</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>STK_Q100</t>
+          <t>TAO_Q100</t>
         </is>
       </c>
       <c r="D84" t="n">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>pMCSKY</t>
+          <t>SOP</t>
         </is>
       </c>
       <c r="F84" t="n">
-        <v>12784.564</v>
+        <v>24047.51666666667</v>
       </c>
       <c r="G84" t="n">
-        <v>121.66</v>
+        <v>231.5</v>
       </c>
       <c r="H84" t="n">
-        <v>157</v>
+        <v>330</v>
       </c>
       <c r="I84" t="n">
-        <v>88.59999999999999</v>
+        <v>122.3333333333333</v>
       </c>
       <c r="J84" t="n">
-        <v>283</v>
+        <v>564</v>
       </c>
     </row>
     <row r="85">
@@ -3650,27 +3650,27 @@
         </is>
       </c>
       <c r="D85" t="n">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>MDUAL</t>
+          <t>pMCSKY</t>
         </is>
       </c>
       <c r="F85" t="n">
-        <v>100.0466666666667</v>
+        <v>23311.61333333333</v>
       </c>
       <c r="G85" t="n">
-        <v>6.099999999999999</v>
+        <v>172.0666666666667</v>
       </c>
       <c r="H85" t="n">
-        <v>16</v>
+        <v>222.3333333333333</v>
       </c>
       <c r="I85" t="n">
-        <v>116</v>
+        <v>122.3333333333333</v>
       </c>
       <c r="J85" t="n">
-        <v>505.6666666666667</v>
+        <v>564</v>
       </c>
     </row>
     <row r="86">
@@ -3688,27 +3688,27 @@
         </is>
       </c>
       <c r="D86" t="n">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>SOP</t>
+          <t>MDUAL</t>
         </is>
       </c>
       <c r="F86" t="n">
-        <v>4565.05</v>
+        <v>115.5</v>
       </c>
       <c r="G86" t="n">
-        <v>228.1</v>
+        <v>6.266666666666667</v>
       </c>
       <c r="H86" t="n">
-        <v>267</v>
+        <v>18</v>
       </c>
       <c r="I86" t="n">
-        <v>116</v>
+        <v>119.3333333333333</v>
       </c>
       <c r="J86" t="n">
-        <v>505.6666666666667</v>
+        <v>554.3333333333334</v>
       </c>
     </row>
     <row r="87">
@@ -3726,27 +3726,27 @@
         </is>
       </c>
       <c r="D87" t="n">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>pMCSKY</t>
+          <t>SOP</t>
         </is>
       </c>
       <c r="F87" t="n">
-        <v>4428.433333333333</v>
+        <v>23679.91</v>
       </c>
       <c r="G87" t="n">
-        <v>186.7666666666667</v>
+        <v>231.4666666666667</v>
       </c>
       <c r="H87" t="n">
-        <v>226</v>
+        <v>279.6666666666667</v>
       </c>
       <c r="I87" t="n">
-        <v>116</v>
+        <v>119.3333333333333</v>
       </c>
       <c r="J87" t="n">
-        <v>505.6666666666667</v>
+        <v>554.3333333333334</v>
       </c>
     </row>
     <row r="88">
@@ -3764,27 +3764,27 @@
         </is>
       </c>
       <c r="D88" t="n">
-        <v>0.2</v>
+        <v>0.8</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>MDUAL</t>
+          <t>pMCSKY</t>
         </is>
       </c>
       <c r="F88" t="n">
-        <v>109.536</v>
+        <v>22931.48333333333</v>
       </c>
       <c r="G88" t="n">
-        <v>6.26</v>
+        <v>171.4</v>
       </c>
       <c r="H88" t="n">
-        <v>18.4</v>
+        <v>244.6666666666667</v>
       </c>
       <c r="I88" t="n">
-        <v>121.6</v>
+        <v>119.3333333333333</v>
       </c>
       <c r="J88" t="n">
-        <v>560.2</v>
+        <v>554.3333333333334</v>
       </c>
     </row>
     <row r="89">
@@ -3802,27 +3802,27 @@
         </is>
       </c>
       <c r="D89" t="n">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>MDUAL-D</t>
+          <t>MDUAL</t>
         </is>
       </c>
       <c r="F89" t="n">
-        <v>678.2499999999999</v>
+        <v>121.505</v>
       </c>
       <c r="G89" t="n">
-        <v>5.4</v>
+        <v>6.2</v>
       </c>
       <c r="H89" t="n">
-        <v>17.6</v>
+        <v>18.5</v>
       </c>
       <c r="I89" t="n">
-        <v>121.6</v>
+        <v>119</v>
       </c>
       <c r="J89" t="n">
-        <v>560.2</v>
+        <v>558.5</v>
       </c>
     </row>
     <row r="90">
@@ -3840,27 +3840,27 @@
         </is>
       </c>
       <c r="D90" t="n">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>MDUAL-Q</t>
+          <t>SOP</t>
         </is>
       </c>
       <c r="F90" t="n">
-        <v>687.472</v>
+        <v>23665.505</v>
       </c>
       <c r="G90" t="n">
-        <v>6.1</v>
+        <v>230.7</v>
       </c>
       <c r="H90" t="n">
-        <v>16</v>
+        <v>280.5</v>
       </c>
       <c r="I90" t="n">
-        <v>121.6</v>
+        <v>119</v>
       </c>
       <c r="J90" t="n">
-        <v>560.2</v>
+        <v>558.5</v>
       </c>
     </row>
     <row r="91">
@@ -3878,444 +3878,26 @@
         </is>
       </c>
       <c r="D91" t="n">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>NAIVE</t>
+          <t>pMCSKY</t>
         </is>
       </c>
       <c r="F91" t="n">
-        <v>15498.722</v>
+        <v>23988.825</v>
       </c>
       <c r="G91" t="n">
-        <v>2</v>
+        <v>170.7</v>
       </c>
       <c r="H91" t="n">
-        <v>12</v>
+        <v>266.5</v>
       </c>
       <c r="I91" t="n">
-        <v>121.6</v>
+        <v>119</v>
       </c>
       <c r="J91" t="n">
-        <v>560.2</v>
-      </c>
-    </row>
-    <row r="92">
-      <c r="A92" s="1" t="n">
-        <v>90</v>
-      </c>
-      <c r="B92" t="inlineStr">
-        <is>
-          <t>TAO</t>
-        </is>
-      </c>
-      <c r="C92" t="inlineStr">
-        <is>
-          <t>TAO_Q100</t>
-        </is>
-      </c>
-      <c r="D92" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="E92" t="inlineStr">
-        <is>
-          <t>SOP</t>
-        </is>
-      </c>
-      <c r="F92" t="n">
-        <v>24179.346</v>
-      </c>
-      <c r="G92" t="n">
-        <v>229.84</v>
-      </c>
-      <c r="H92" t="n">
-        <v>279.2</v>
-      </c>
-      <c r="I92" t="n">
-        <v>121.6</v>
-      </c>
-      <c r="J92" t="n">
-        <v>560.2</v>
-      </c>
-    </row>
-    <row r="93">
-      <c r="A93" s="1" t="n">
-        <v>91</v>
-      </c>
-      <c r="B93" t="inlineStr">
-        <is>
-          <t>TAO</t>
-        </is>
-      </c>
-      <c r="C93" t="inlineStr">
-        <is>
-          <t>TAO_Q100</t>
-        </is>
-      </c>
-      <c r="D93" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="E93" t="inlineStr">
-        <is>
-          <t>pMCSKY</t>
-        </is>
-      </c>
-      <c r="F93" t="n">
-        <v>23755.652</v>
-      </c>
-      <c r="G93" t="n">
-        <v>170.6</v>
-      </c>
-      <c r="H93" t="n">
-        <v>220</v>
-      </c>
-      <c r="I93" t="n">
-        <v>121.6</v>
-      </c>
-      <c r="J93" t="n">
-        <v>560.2</v>
-      </c>
-    </row>
-    <row r="94">
-      <c r="A94" s="1" t="n">
-        <v>92</v>
-      </c>
-      <c r="B94" t="inlineStr">
-        <is>
-          <t>TAO</t>
-        </is>
-      </c>
-      <c r="C94" t="inlineStr">
-        <is>
-          <t>TAO_Q100</t>
-        </is>
-      </c>
-      <c r="D94" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="E94" t="inlineStr">
-        <is>
-          <t>MDUAL</t>
-        </is>
-      </c>
-      <c r="F94" t="n">
-        <v>117.3966666666667</v>
-      </c>
-      <c r="G94" t="n">
-        <v>6.333333333333333</v>
-      </c>
-      <c r="H94" t="n">
-        <v>19</v>
-      </c>
-      <c r="I94" t="n">
-        <v>122.3333333333333</v>
-      </c>
-      <c r="J94" t="n">
-        <v>564</v>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95" s="1" t="n">
-        <v>93</v>
-      </c>
-      <c r="B95" t="inlineStr">
-        <is>
-          <t>TAO</t>
-        </is>
-      </c>
-      <c r="C95" t="inlineStr">
-        <is>
-          <t>TAO_Q100</t>
-        </is>
-      </c>
-      <c r="D95" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="E95" t="inlineStr">
-        <is>
-          <t>SOP</t>
-        </is>
-      </c>
-      <c r="F95" t="n">
-        <v>24047.51666666667</v>
-      </c>
-      <c r="G95" t="n">
-        <v>231.5</v>
-      </c>
-      <c r="H95" t="n">
-        <v>330</v>
-      </c>
-      <c r="I95" t="n">
-        <v>122.3333333333333</v>
-      </c>
-      <c r="J95" t="n">
-        <v>564</v>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96" s="1" t="n">
-        <v>94</v>
-      </c>
-      <c r="B96" t="inlineStr">
-        <is>
-          <t>TAO</t>
-        </is>
-      </c>
-      <c r="C96" t="inlineStr">
-        <is>
-          <t>TAO_Q100</t>
-        </is>
-      </c>
-      <c r="D96" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="E96" t="inlineStr">
-        <is>
-          <t>pMCSKY</t>
-        </is>
-      </c>
-      <c r="F96" t="n">
-        <v>23311.61333333333</v>
-      </c>
-      <c r="G96" t="n">
-        <v>172.0666666666667</v>
-      </c>
-      <c r="H96" t="n">
-        <v>222.3333333333333</v>
-      </c>
-      <c r="I96" t="n">
-        <v>122.3333333333333</v>
-      </c>
-      <c r="J96" t="n">
-        <v>564</v>
-      </c>
-    </row>
-    <row r="97">
-      <c r="A97" s="1" t="n">
-        <v>95</v>
-      </c>
-      <c r="B97" t="inlineStr">
-        <is>
-          <t>TAO</t>
-        </is>
-      </c>
-      <c r="C97" t="inlineStr">
-        <is>
-          <t>TAO_Q100</t>
-        </is>
-      </c>
-      <c r="D97" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="E97" t="inlineStr">
-        <is>
-          <t>MDUAL</t>
-        </is>
-      </c>
-      <c r="F97" t="n">
-        <v>115.5</v>
-      </c>
-      <c r="G97" t="n">
-        <v>6.266666666666667</v>
-      </c>
-      <c r="H97" t="n">
-        <v>18</v>
-      </c>
-      <c r="I97" t="n">
-        <v>119.3333333333333</v>
-      </c>
-      <c r="J97" t="n">
-        <v>554.3333333333334</v>
-      </c>
-    </row>
-    <row r="98">
-      <c r="A98" s="1" t="n">
-        <v>96</v>
-      </c>
-      <c r="B98" t="inlineStr">
-        <is>
-          <t>TAO</t>
-        </is>
-      </c>
-      <c r="C98" t="inlineStr">
-        <is>
-          <t>TAO_Q100</t>
-        </is>
-      </c>
-      <c r="D98" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="E98" t="inlineStr">
-        <is>
-          <t>SOP</t>
-        </is>
-      </c>
-      <c r="F98" t="n">
-        <v>23679.91</v>
-      </c>
-      <c r="G98" t="n">
-        <v>231.4666666666667</v>
-      </c>
-      <c r="H98" t="n">
-        <v>279.6666666666667</v>
-      </c>
-      <c r="I98" t="n">
-        <v>119.3333333333333</v>
-      </c>
-      <c r="J98" t="n">
-        <v>554.3333333333334</v>
-      </c>
-    </row>
-    <row r="99">
-      <c r="A99" s="1" t="n">
-        <v>97</v>
-      </c>
-      <c r="B99" t="inlineStr">
-        <is>
-          <t>TAO</t>
-        </is>
-      </c>
-      <c r="C99" t="inlineStr">
-        <is>
-          <t>TAO_Q100</t>
-        </is>
-      </c>
-      <c r="D99" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="E99" t="inlineStr">
-        <is>
-          <t>pMCSKY</t>
-        </is>
-      </c>
-      <c r="F99" t="n">
-        <v>22931.48333333333</v>
-      </c>
-      <c r="G99" t="n">
-        <v>171.4</v>
-      </c>
-      <c r="H99" t="n">
-        <v>244.6666666666667</v>
-      </c>
-      <c r="I99" t="n">
-        <v>119.3333333333333</v>
-      </c>
-      <c r="J99" t="n">
-        <v>554.3333333333334</v>
-      </c>
-    </row>
-    <row r="100">
-      <c r="A100" s="1" t="n">
-        <v>98</v>
-      </c>
-      <c r="B100" t="inlineStr">
-        <is>
-          <t>TAO</t>
-        </is>
-      </c>
-      <c r="C100" t="inlineStr">
-        <is>
-          <t>TAO_Q100</t>
-        </is>
-      </c>
-      <c r="D100" t="n">
-        <v>1</v>
-      </c>
-      <c r="E100" t="inlineStr">
-        <is>
-          <t>MDUAL</t>
-        </is>
-      </c>
-      <c r="F100" t="n">
-        <v>121.505</v>
-      </c>
-      <c r="G100" t="n">
-        <v>6.2</v>
-      </c>
-      <c r="H100" t="n">
-        <v>18.5</v>
-      </c>
-      <c r="I100" t="n">
-        <v>119</v>
-      </c>
-      <c r="J100" t="n">
-        <v>558.5</v>
-      </c>
-    </row>
-    <row r="101">
-      <c r="A101" s="1" t="n">
-        <v>99</v>
-      </c>
-      <c r="B101" t="inlineStr">
-        <is>
-          <t>TAO</t>
-        </is>
-      </c>
-      <c r="C101" t="inlineStr">
-        <is>
-          <t>TAO_Q100</t>
-        </is>
-      </c>
-      <c r="D101" t="n">
-        <v>1</v>
-      </c>
-      <c r="E101" t="inlineStr">
-        <is>
-          <t>SOP</t>
-        </is>
-      </c>
-      <c r="F101" t="n">
-        <v>23665.505</v>
-      </c>
-      <c r="G101" t="n">
-        <v>230.7</v>
-      </c>
-      <c r="H101" t="n">
-        <v>280.5</v>
-      </c>
-      <c r="I101" t="n">
-        <v>119</v>
-      </c>
-      <c r="J101" t="n">
-        <v>558.5</v>
-      </c>
-    </row>
-    <row r="102">
-      <c r="A102" s="1" t="n">
-        <v>100</v>
-      </c>
-      <c r="B102" t="inlineStr">
-        <is>
-          <t>TAO</t>
-        </is>
-      </c>
-      <c r="C102" t="inlineStr">
-        <is>
-          <t>TAO_Q100</t>
-        </is>
-      </c>
-      <c r="D102" t="n">
-        <v>1</v>
-      </c>
-      <c r="E102" t="inlineStr">
-        <is>
-          <t>pMCSKY</t>
-        </is>
-      </c>
-      <c r="F102" t="n">
-        <v>23988.825</v>
-      </c>
-      <c r="G102" t="n">
-        <v>170.7</v>
-      </c>
-      <c r="H102" t="n">
-        <v>266.5</v>
-      </c>
-      <c r="I102" t="n">
-        <v>119</v>
-      </c>
-      <c r="J102" t="n">
         <v>558.5</v>
       </c>
     </row>

</xml_diff>